<commit_message>
Checkpoint: Successful file access from HTML button
</commit_message>
<xml_diff>
--- a/SendMessage_Testing.xlsx
+++ b/SendMessage_Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\3D_Viz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345FB77B-8F7B-43A2-BB20-695B1B2CB1F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22011E16-00B4-4CDF-9BE6-D89D7A254E29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4452" xr2:uid="{0F8D62C4-D090-4D7A-BF59-AC759E9B056E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>BrowserFileDialog</t>
   </si>
@@ -48,16 +48,58 @@
     <t>"1"; URL; "5"</t>
   </si>
   <si>
-    <t>Debug.Log</t>
-  </si>
-  <si>
     <t>Python server</t>
   </si>
   <si>
-    <t>Gchrome</t>
-  </si>
-  <si>
     <t>FireFox</t>
+  </si>
+  <si>
+    <t>GZIP</t>
+  </si>
+  <si>
+    <t>GChrome</t>
+  </si>
+  <si>
+    <t>Build time</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>File Sent</t>
+  </si>
+  <si>
+    <t>Test.txt</t>
+  </si>
+  <si>
+    <t>The Mom Test.docx</t>
+  </si>
+  <si>
+    <t>Carp DS (csv)</t>
+  </si>
+  <si>
+    <t>Debug.Log(fileurl)</t>
+  </si>
+  <si>
+    <t>Debug.Log(UrlTextField.text)</t>
+  </si>
+  <si>
+    <t>Full coroutine; UrlTextField.text disabled</t>
+  </si>
+  <si>
+    <t>Test.csv</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Ran out of memory in attempting to print</t>
+  </si>
+  <si>
+    <t>Coroutine w/out printing file contents; UrlTextField.text disabled</t>
+  </si>
+  <si>
+    <t>Coroutine; prints type (string) and length (15M)</t>
   </si>
 </sst>
 </file>
@@ -93,8 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,18 +454,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E806C3-7404-4F3D-A8C2-C610700761F1}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="10" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,18 +486,27 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -471,11 +526,352 @@
       <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
       <c r="I2" t="b">
         <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>